<commit_message>
Primeira reunião para definição de ações
</commit_message>
<xml_diff>
--- a/00_Planejamento/Burndown.xlsx
+++ b/00_Planejamento/Burndown.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8e9917896f9ae4b2/Pessoal/Documents/PIM/4º Semestre/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sandbox\github\pim-condominio\00_Planejamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="C952CE0B6C4B244A6163F46833DA469644A06B34" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{0EC1470F-8C4B-4883-A4C1-B3F76B9916E7}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7650" xr2:uid="{47731978-CD95-4883-A0E8-27557D7E7242}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7650" activeTab="1" xr2:uid="{47731978-CD95-4883-A0E8-27557D7E7242}"/>
   </bookViews>
   <sheets>
     <sheet name="Legendas" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="61">
   <si>
     <t>Prioridades</t>
   </si>
@@ -131,13 +130,91 @@
   </si>
   <si>
     <t>Carlos Bezerra Silva</t>
+  </si>
+  <si>
+    <t>Análise</t>
+  </si>
+  <si>
+    <t>PIM</t>
+  </si>
+  <si>
+    <t>Inserir PIM do 3º Semestre para ser utilizado como base do Projeto</t>
+  </si>
+  <si>
+    <t>Diagrama</t>
+  </si>
+  <si>
+    <t>Diagrama de Classes</t>
+  </si>
+  <si>
+    <t>Definir requisitos necessários para criar Diagrama</t>
+  </si>
+  <si>
+    <t>Diagrama de Sequencia</t>
+  </si>
+  <si>
+    <t>Diagrama de Máquina de Estados</t>
+  </si>
+  <si>
+    <t>Diagrama de Comunicação</t>
+  </si>
+  <si>
+    <t>Diagrama de Pacotes</t>
+  </si>
+  <si>
+    <t>Haverá inclusão de Tarefas para esta atividade</t>
+  </si>
+  <si>
+    <t>Modelo de Dados</t>
+  </si>
+  <si>
+    <t>MER</t>
+  </si>
+  <si>
+    <t>Apresentar Modelo de Dados Normalizado</t>
+  </si>
+  <si>
+    <t>Arquitetura</t>
+  </si>
+  <si>
+    <t>Arquitetura de Sistemas</t>
+  </si>
+  <si>
+    <t>Definir ações para criação de arquitetura</t>
+  </si>
+  <si>
+    <t>Estudos</t>
+  </si>
+  <si>
+    <t>Empreendimento</t>
+  </si>
+  <si>
+    <t>Definir Estudo de Empreendimento na área de desenvolvimento de Sistemas</t>
+  </si>
+  <si>
+    <t>Testes</t>
+  </si>
+  <si>
+    <t>Qualidade</t>
+  </si>
+  <si>
+    <t>Definir informações sobre controle de qualidade utilizado na produção do sistema</t>
+  </si>
+  <si>
+    <t>Cronogramas</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Definir Cronogramas de Projeto</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +224,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -369,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -386,15 +471,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -407,24 +483,32 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="99">
+  <dxfs count="15">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -510,601 +594,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF99CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF99CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF99CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF99CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF99CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF99CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF99CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF99CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF99CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF99CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF99CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF99CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF99CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF99CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1131,14 +620,14 @@
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{A175D227-A97C-47C3-AD56-66B3A2A41D22}" name="Categoria"/>
     <tableColumn id="2" xr3:uid="{0029B6F2-8F22-47FD-AA27-DEE55C28308D}" name="Sub-Categoria"/>
-    <tableColumn id="3" xr3:uid="{B7CB9F69-9160-4984-B559-E59BDBBE88F9}" name="Descrição"/>
+    <tableColumn id="3" xr3:uid="{B7CB9F69-9160-4984-B559-E59BDBBE88F9}" name="Descrição" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{05D307D3-E407-4E78-B4D3-E0C2D5AD7278}" name="Responsável"/>
     <tableColumn id="5" xr3:uid="{F32CE024-6A09-42EF-82A5-C626594D402F}" name="Prioridade"/>
     <tableColumn id="6" xr3:uid="{40F18E8C-1404-4891-9C73-2EBB2BCF43EA}" name="Dificuldade"/>
     <tableColumn id="7" xr3:uid="{77CE48E1-7F83-4B2A-83E3-47D04AE53DAF}" name="OK / NOK"/>
     <tableColumn id="8" xr3:uid="{1B0E619C-FE57-4789-901D-BEBE0F1B3CFD}" name="Data de Conclusão"/>
-    <tableColumn id="9" xr3:uid="{5D2FE0D6-C372-43E7-B2BE-4D80CCC54FE6}" name="Dúvidas"/>
-    <tableColumn id="10" xr3:uid="{BED6E019-A917-4461-BD4D-284EF2827FA2}" name="Obs"/>
+    <tableColumn id="9" xr3:uid="{5D2FE0D6-C372-43E7-B2BE-4D80CCC54FE6}" name="Dúvidas" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{BED6E019-A917-4461-BD4D-284EF2827FA2}" name="Obs" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1443,7 +932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D295075-4551-48AA-B4AB-DAE61E022DF5}">
   <dimension ref="B1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -1457,34 +946,34 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="20" t="s">
         <v>29</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="17" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="15"/>
-      <c r="C3" s="18" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="15" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="15"/>
+      <c r="G3" s="21"/>
       <c r="H3" s="12" t="s">
         <v>25</v>
       </c>
@@ -1493,14 +982,14 @@
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="15"/>
-      <c r="C4" s="18" t="s">
+      <c r="B4" s="21"/>
+      <c r="C4" s="15" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="15"/>
+      <c r="G4" s="21"/>
       <c r="H4" s="12" t="s">
         <v>26</v>
       </c>
@@ -1509,14 +998,14 @@
       </c>
     </row>
     <row r="5" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="16"/>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="15"/>
+      <c r="G5" s="21"/>
       <c r="H5" s="12" t="s">
         <v>27</v>
       </c>
@@ -1525,7 +1014,7 @@
       </c>
     </row>
     <row r="6" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G6" s="16"/>
+      <c r="G6" s="22"/>
       <c r="H6" s="13" t="s">
         <v>28</v>
       </c>
@@ -1534,19 +1023,19 @@
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
-      <c r="C8" s="18" t="s">
+      <c r="B8" s="21"/>
+      <c r="C8" s="15" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -1554,11 +1043,11 @@
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="16"/>
-      <c r="C9" s="19" t="s">
+      <c r="B9" s="22"/>
+      <c r="C9" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="19" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1575,24 +1064,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{777211D6-37A4-41E9-8C16-55AAF1157B83}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.7109375" style="23" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" customWidth="1"/>
-    <col min="10" max="10" width="29" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.7109375" style="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1602,7 +1091,7 @@
       <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="23" t="s">
         <v>17</v>
       </c>
       <c r="D1" t="s">
@@ -1620,17 +1109,247 @@
       <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="23" t="s">
         <v>23</v>
       </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">

</xml_diff>

<commit_message>
Inclusão de tarefas de desenvolvimento
</commit_message>
<xml_diff>
--- a/00_Planejamento/Burndown.xlsx
+++ b/00_Planejamento/Burndown.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="105">
   <si>
     <t>Prioridades</t>
   </si>
@@ -208,13 +208,145 @@
   </si>
   <si>
     <t>Definir Cronogramas de Projeto</t>
+  </si>
+  <si>
+    <t>Desenvolvimento</t>
+  </si>
+  <si>
+    <t>CRUD</t>
+  </si>
+  <si>
+    <t>Morador</t>
+  </si>
+  <si>
+    <t>Dependentes</t>
+  </si>
+  <si>
+    <t>Aluguel</t>
+  </si>
+  <si>
+    <t>Apartamento</t>
+  </si>
+  <si>
+    <t>Contrato</t>
+  </si>
+  <si>
+    <t>Estacionamento</t>
+  </si>
+  <si>
+    <t>Ocorrência</t>
+  </si>
+  <si>
+    <t>Tipo Reserva</t>
+  </si>
+  <si>
+    <t>Reserva</t>
+  </si>
+  <si>
+    <t>Grupo Usuário</t>
+  </si>
+  <si>
+    <t>Permissão de Acesso</t>
+  </si>
+  <si>
+    <t>Colaborador</t>
+  </si>
+  <si>
+    <t>Usuário</t>
+  </si>
+  <si>
+    <t>Buscas Win Forms</t>
+  </si>
+  <si>
+    <t>Dependente</t>
+  </si>
+  <si>
+    <t>Buscas Web</t>
+  </si>
+  <si>
+    <t>Projeto</t>
+  </si>
+  <si>
+    <t>Criar Projeto CRUD - Database</t>
+  </si>
+  <si>
+    <t>Criar Projeto Services</t>
+  </si>
+  <si>
+    <t>Criar Projeto WEB</t>
+  </si>
+  <si>
+    <t>Criar Projeto Win Forms</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>Implementar Métodos de Crud</t>
+  </si>
+  <si>
+    <t>Win Forms</t>
+  </si>
+  <si>
+    <t>Criar Formulario CRUD Morador</t>
+  </si>
+  <si>
+    <t>Criar Formulario CRUD Dependente</t>
+  </si>
+  <si>
+    <t>Criar Formulario CRUD Aluguel</t>
+  </si>
+  <si>
+    <t>Criar Formulario CRUD Apartamento</t>
+  </si>
+  <si>
+    <t>Criar Formulario CRUD Contrato</t>
+  </si>
+  <si>
+    <t>Criar Formulario CRUD Estacionamento</t>
+  </si>
+  <si>
+    <t>Criar Formulario CRUD Ocorrência</t>
+  </si>
+  <si>
+    <t>Criar Formulario CRUD Tipo Reserva</t>
+  </si>
+  <si>
+    <t>Criar Formulario CRUD Reserva</t>
+  </si>
+  <si>
+    <t>Criar Formulario CRUD Grupo Usuário</t>
+  </si>
+  <si>
+    <t>Criar Formulario CRUD Permissão de Acesso</t>
+  </si>
+  <si>
+    <t>Criar Formulario CRUD Colaborador</t>
+  </si>
+  <si>
+    <t>Criar Formulario CRUD Usuário</t>
+  </si>
+  <si>
+    <t>Incluir tratamentos de strings, exceções, erros e mensagens</t>
+  </si>
+  <si>
+    <t>Definir armazenamento de senha</t>
+  </si>
+  <si>
+    <t>Se houver mudança de estrutura na senha (Ex: HASH) alterará no modelo de dados</t>
+  </si>
+  <si>
+    <t>Revisão</t>
+  </si>
+  <si>
+    <t>Revisar e readequar modelo de dados</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -224,14 +356,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -483,6 +607,9 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -492,56 +619,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -562,7 +649,49 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF99CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4"/>
         </patternFill>
       </fill>
     </dxf>
@@ -576,23 +705,18 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4"/>
+          <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF99CC"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -615,19 +739,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B615B5C8-D8E7-4A77-806A-F0D05B67BCD9}" name="Alteracoes" displayName="Alteracoes" ref="A1:J27" totalsRowShown="0">
-  <autoFilter ref="A1:J27" xr:uid="{5AA77EDB-A50A-476C-9B8A-65586C6DAE69}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B615B5C8-D8E7-4A77-806A-F0D05B67BCD9}" name="Alteracoes" displayName="Alteracoes" ref="A1:J85" totalsRowShown="0">
+  <autoFilter ref="A1:J85" xr:uid="{5AA77EDB-A50A-476C-9B8A-65586C6DAE69}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{A175D227-A97C-47C3-AD56-66B3A2A41D22}" name="Categoria"/>
     <tableColumn id="2" xr3:uid="{0029B6F2-8F22-47FD-AA27-DEE55C28308D}" name="Sub-Categoria"/>
-    <tableColumn id="3" xr3:uid="{B7CB9F69-9160-4984-B559-E59BDBBE88F9}" name="Descrição" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{B7CB9F69-9160-4984-B559-E59BDBBE88F9}" name="Descrição" dataDxfId="14"/>
     <tableColumn id="4" xr3:uid="{05D307D3-E407-4E78-B4D3-E0C2D5AD7278}" name="Responsável"/>
     <tableColumn id="5" xr3:uid="{F32CE024-6A09-42EF-82A5-C626594D402F}" name="Prioridade"/>
     <tableColumn id="6" xr3:uid="{40F18E8C-1404-4891-9C73-2EBB2BCF43EA}" name="Dificuldade"/>
     <tableColumn id="7" xr3:uid="{77CE48E1-7F83-4B2A-83E3-47D04AE53DAF}" name="OK / NOK"/>
     <tableColumn id="8" xr3:uid="{1B0E619C-FE57-4789-901D-BEBE0F1B3CFD}" name="Data de Conclusão"/>
-    <tableColumn id="9" xr3:uid="{5D2FE0D6-C372-43E7-B2BE-4D80CCC54FE6}" name="Dúvidas" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{BED6E019-A917-4461-BD4D-284EF2827FA2}" name="Obs" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{5D2FE0D6-C372-43E7-B2BE-4D80CCC54FE6}" name="Dúvidas" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{BED6E019-A917-4461-BD4D-284EF2827FA2}" name="Obs" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -946,7 +1070,7 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="14" t="s">
@@ -955,7 +1079,7 @@
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="21" t="s">
         <v>29</v>
       </c>
       <c r="H2" s="11" t="s">
@@ -966,14 +1090,14 @@
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="21"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="15" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="21"/>
+      <c r="G3" s="22"/>
       <c r="H3" s="12" t="s">
         <v>25</v>
       </c>
@@ -982,14 +1106,14 @@
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="21"/>
+      <c r="B4" s="22"/>
       <c r="C4" s="15" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="21"/>
+      <c r="G4" s="22"/>
       <c r="H4" s="12" t="s">
         <v>26</v>
       </c>
@@ -998,14 +1122,14 @@
       </c>
     </row>
     <row r="5" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="22"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="21"/>
+      <c r="G5" s="22"/>
       <c r="H5" s="12" t="s">
         <v>27</v>
       </c>
@@ -1014,7 +1138,7 @@
       </c>
     </row>
     <row r="6" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G6" s="22"/>
+      <c r="G6" s="23"/>
       <c r="H6" s="13" t="s">
         <v>28</v>
       </c>
@@ -1023,7 +1147,7 @@
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="21" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="14" t="s">
@@ -1034,7 +1158,7 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="21"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="15" t="s">
         <v>2</v>
       </c>
@@ -1043,7 +1167,7 @@
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="22"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="16" t="s">
         <v>7</v>
       </c>
@@ -1064,24 +1188,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{777211D6-37A4-41E9-8C16-55AAF1157B83}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.7109375" style="23" customWidth="1"/>
+    <col min="3" max="3" width="65.140625" style="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" style="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="42.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42.7109375" style="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1091,7 +1215,7 @@
       <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D1" t="s">
@@ -1109,10 +1233,10 @@
       <c r="H1" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="20" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1123,7 +1247,7 @@
       <c r="B2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="20" t="s">
         <v>37</v>
       </c>
       <c r="D2" t="s">
@@ -1143,7 +1267,7 @@
       <c r="B3" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="20" t="s">
         <v>40</v>
       </c>
       <c r="D3" t="s">
@@ -1155,7 +1279,7 @@
       <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="J3" s="20" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1166,7 +1290,7 @@
       <c r="B4" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="20" t="s">
         <v>40</v>
       </c>
       <c r="D4" t="s">
@@ -1178,7 +1302,7 @@
       <c r="F4" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="23" t="s">
+      <c r="J4" s="20" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1189,7 +1313,7 @@
       <c r="B5" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="20" t="s">
         <v>40</v>
       </c>
       <c r="D5" t="s">
@@ -1201,7 +1325,7 @@
       <c r="F5" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="23" t="s">
+      <c r="J5" s="20" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1212,7 +1336,7 @@
       <c r="B6" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="20" t="s">
         <v>40</v>
       </c>
       <c r="D6" t="s">
@@ -1224,7 +1348,7 @@
       <c r="F6" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="J6" s="20" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1235,7 +1359,7 @@
       <c r="B7" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="20" t="s">
         <v>40</v>
       </c>
       <c r="D7" t="s">
@@ -1247,7 +1371,7 @@
       <c r="F7" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="23" t="s">
+      <c r="J7" s="20" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1258,7 +1382,7 @@
       <c r="B8" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="20" t="s">
         <v>48</v>
       </c>
       <c r="D8" t="s">
@@ -1278,7 +1402,7 @@
       <c r="B9" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="20" t="s">
         <v>51</v>
       </c>
       <c r="D9" t="s">
@@ -1298,7 +1422,7 @@
       <c r="B10" t="s">
         <v>53</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="20" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1309,7 +1433,7 @@
       <c r="B11" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="20" t="s">
         <v>57</v>
       </c>
       <c r="D11" t="s">
@@ -1329,7 +1453,7 @@
       <c r="B12" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="20" t="s">
         <v>60</v>
       </c>
       <c r="D12" t="s">
@@ -1343,7 +1467,1066 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" t="s">
+        <v>27</v>
+      </c>
+      <c r="E32" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" t="s">
+        <v>27</v>
+      </c>
+      <c r="E34" t="s">
+        <v>2</v>
+      </c>
+      <c r="F34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" t="s">
+        <v>27</v>
+      </c>
+      <c r="E35" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D36" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" t="s">
+        <v>2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" t="s">
+        <v>2</v>
+      </c>
+      <c r="F40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" t="s">
+        <v>78</v>
+      </c>
+      <c r="C41" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D41" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" t="s">
+        <v>2</v>
+      </c>
+      <c r="F41" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D42" t="s">
+        <v>25</v>
+      </c>
+      <c r="E42" t="s">
+        <v>2</v>
+      </c>
+      <c r="F42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" t="s">
+        <v>25</v>
+      </c>
+      <c r="E43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D44" t="s">
+        <v>25</v>
+      </c>
+      <c r="E44" t="s">
+        <v>2</v>
+      </c>
+      <c r="F44" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D45" t="s">
+        <v>25</v>
+      </c>
+      <c r="E45" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D46" t="s">
+        <v>25</v>
+      </c>
+      <c r="E46" t="s">
+        <v>2</v>
+      </c>
+      <c r="F46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D47" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" t="s">
+        <v>2</v>
+      </c>
+      <c r="F47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>61</v>
+      </c>
+      <c r="B48" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D48" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" t="s">
+        <v>2</v>
+      </c>
+      <c r="F48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49" t="s">
+        <v>86</v>
+      </c>
+      <c r="C49" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D49" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" t="s">
+        <v>2</v>
+      </c>
+      <c r="F49" t="s">
+        <v>2</v>
+      </c>
+      <c r="J49" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>61</v>
+      </c>
+      <c r="B50" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="D50" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" t="s">
+        <v>2</v>
+      </c>
+      <c r="F50" t="s">
+        <v>2</v>
+      </c>
+      <c r="J50" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>61</v>
+      </c>
+      <c r="B51" t="s">
+        <v>86</v>
+      </c>
+      <c r="C51" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D51" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" t="s">
+        <v>2</v>
+      </c>
+      <c r="F51" t="s">
+        <v>2</v>
+      </c>
+      <c r="J51" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>61</v>
+      </c>
+      <c r="B52" t="s">
+        <v>86</v>
+      </c>
+      <c r="C52" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D52" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" t="s">
+        <v>2</v>
+      </c>
+      <c r="F52" t="s">
+        <v>2</v>
+      </c>
+      <c r="J52" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53" t="s">
+        <v>86</v>
+      </c>
+      <c r="C53" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D53" t="s">
+        <v>27</v>
+      </c>
+      <c r="E53" t="s">
+        <v>2</v>
+      </c>
+      <c r="F53" t="s">
+        <v>2</v>
+      </c>
+      <c r="J53" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54" t="s">
+        <v>86</v>
+      </c>
+      <c r="C54" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D54" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54" t="s">
+        <v>2</v>
+      </c>
+      <c r="F54" t="s">
+        <v>2</v>
+      </c>
+      <c r="J54" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>61</v>
+      </c>
+      <c r="B55" t="s">
+        <v>86</v>
+      </c>
+      <c r="C55" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D55" t="s">
+        <v>27</v>
+      </c>
+      <c r="E55" t="s">
+        <v>2</v>
+      </c>
+      <c r="F55" t="s">
+        <v>2</v>
+      </c>
+      <c r="J55" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56" t="s">
+        <v>86</v>
+      </c>
+      <c r="C56" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D56" t="s">
+        <v>26</v>
+      </c>
+      <c r="E56" t="s">
+        <v>2</v>
+      </c>
+      <c r="F56" t="s">
+        <v>2</v>
+      </c>
+      <c r="J56" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>61</v>
+      </c>
+      <c r="B57" t="s">
+        <v>86</v>
+      </c>
+      <c r="C57" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D57" t="s">
+        <v>26</v>
+      </c>
+      <c r="E57" t="s">
+        <v>2</v>
+      </c>
+      <c r="F57" t="s">
+        <v>2</v>
+      </c>
+      <c r="J57" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58" t="s">
+        <v>86</v>
+      </c>
+      <c r="C58" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D58" t="s">
+        <v>26</v>
+      </c>
+      <c r="E58" t="s">
+        <v>2</v>
+      </c>
+      <c r="F58" t="s">
+        <v>2</v>
+      </c>
+      <c r="J58" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" t="s">
+        <v>86</v>
+      </c>
+      <c r="C59" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D59" t="s">
+        <v>26</v>
+      </c>
+      <c r="E59" t="s">
+        <v>2</v>
+      </c>
+      <c r="F59" t="s">
+        <v>2</v>
+      </c>
+      <c r="J59" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60" t="s">
+        <v>86</v>
+      </c>
+      <c r="C60" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="D60" t="s">
+        <v>26</v>
+      </c>
+      <c r="E60" t="s">
+        <v>2</v>
+      </c>
+      <c r="F60" t="s">
+        <v>2</v>
+      </c>
+      <c r="J60" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" t="s">
+        <v>86</v>
+      </c>
+      <c r="C61" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="D61" t="s">
+        <v>26</v>
+      </c>
+      <c r="E61" t="s">
+        <v>2</v>
+      </c>
+      <c r="F61" t="s">
+        <v>2</v>
+      </c>
+      <c r="J61" s="20" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>79</v>
+      </c>
+      <c r="C62" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D62" t="s">
+        <v>25</v>
+      </c>
+      <c r="E62" t="s">
+        <v>3</v>
+      </c>
+      <c r="F62" t="s">
+        <v>2</v>
+      </c>
+      <c r="J62" s="20" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>46</v>
+      </c>
+      <c r="B63" t="s">
+        <v>103</v>
+      </c>
+      <c r="C63" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D63" t="s">
+        <v>25</v>
+      </c>
+      <c r="E63" t="s">
+        <v>3</v>
+      </c>
+      <c r="F63" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1355,13 +2538,35 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{3A766EC7-076F-4FB4-906B-E1E45593F355}">
-            <xm:f>NOT(ISERROR(SEARCH(Legendas!$H$2,D2)))</xm:f>
-            <xm:f>Legendas!$H$2</xm:f>
+          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{78635B85-74E4-47C4-8108-E73B6C640B83}">
+            <xm:f>NOT(ISERROR(SEARCH(Legendas!$H$6,D2)))</xm:f>
+            <xm:f>Legendas!$H$6</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
-                  <bgColor rgb="FFFF99CC"/>
+                  <bgColor theme="0" tint="-0.499984740745262"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{DE871BE2-C2F2-4691-817F-318AB363F660}">
+            <xm:f>NOT(ISERROR(SEARCH(Legendas!$H$5,D2)))</xm:f>
+            <xm:f>Legendas!$H$5</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF7030A0"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="11" operator="containsText" id="{5DC4C7B5-AFEA-4BEB-9FC4-119FE6DC365B}">
+            <xm:f>NOT(ISERROR(SEARCH(Legendas!$H$4,D2)))</xm:f>
+            <xm:f>Legendas!$H$4</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="4"/>
                 </patternFill>
               </fill>
             </x14:dxf>
@@ -1377,49 +2582,38 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="11" operator="containsText" id="{5DC4C7B5-AFEA-4BEB-9FC4-119FE6DC365B}">
-            <xm:f>NOT(ISERROR(SEARCH(Legendas!$H$4,D2)))</xm:f>
-            <xm:f>Legendas!$H$4</xm:f>
+          <x14:cfRule type="containsText" priority="13" operator="containsText" id="{3A766EC7-076F-4FB4-906B-E1E45593F355}">
+            <xm:f>NOT(ISERROR(SEARCH(Legendas!$H$2,D2)))</xm:f>
+            <xm:f>Legendas!$H$2</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
-                  <bgColor theme="4"/>
+                  <bgColor rgb="FFFF99CC"/>
                 </patternFill>
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{DE871BE2-C2F2-4691-817F-318AB363F660}">
-            <xm:f>NOT(ISERROR(SEARCH(Legendas!$H$5,D2)))</xm:f>
-            <xm:f>Legendas!$H$5</xm:f>
+          <xm:sqref>D2:D85</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{53791CF5-621D-4B81-8AAA-F7386AE0B7DA}">
+            <xm:f>NOT(ISERROR(SEARCH(Legendas!$C$5,E2)))</xm:f>
+            <xm:f>Legendas!$C$5</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
-                  <bgColor rgb="FF7030A0"/>
+                  <bgColor rgb="FF92D050"/>
                 </patternFill>
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="9" operator="containsText" id="{78635B85-74E4-47C4-8108-E73B6C640B83}">
-            <xm:f>NOT(ISERROR(SEARCH(Legendas!$H$6,D2)))</xm:f>
-            <xm:f>Legendas!$H$6</xm:f>
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{DC2230C3-1FC4-4649-A3A7-171330916009}">
+            <xm:f>NOT(ISERROR(SEARCH(Legendas!$C$4,E2)))</xm:f>
+            <xm:f>Legendas!$C$4</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
-                  <bgColor theme="0" tint="-0.499984740745262"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>D2:D27</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{689F638C-F03D-4CAC-B35D-E2AA229A5899}">
-            <xm:f>NOT(ISERROR(SEARCH(Legendas!$C$2,E2)))</xm:f>
-            <xm:f>Legendas!$C$2</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFF0000"/>
+                  <bgColor rgb="FFFFFF00"/>
                 </patternFill>
               </fill>
             </x14:dxf>
@@ -1435,38 +2629,27 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{DC2230C3-1FC4-4649-A3A7-171330916009}">
-            <xm:f>NOT(ISERROR(SEARCH(Legendas!$C$4,E2)))</xm:f>
-            <xm:f>Legendas!$C$4</xm:f>
+          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{689F638C-F03D-4CAC-B35D-E2AA229A5899}">
+            <xm:f>NOT(ISERROR(SEARCH(Legendas!$C$2,E2)))</xm:f>
+            <xm:f>Legendas!$C$2</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
-                  <bgColor rgb="FFFFFF00"/>
+                  <bgColor rgb="FFFF0000"/>
                 </patternFill>
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{53791CF5-621D-4B81-8AAA-F7386AE0B7DA}">
-            <xm:f>NOT(ISERROR(SEARCH(Legendas!$C$5,E2)))</xm:f>
-            <xm:f>Legendas!$C$5</xm:f>
+          <xm:sqref>E2:E85</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{247A90A8-51E8-41C3-9472-4F7E573E1980}">
+            <xm:f>NOT(ISERROR(SEARCH(Legendas!$C$9,F2)))</xm:f>
+            <xm:f>Legendas!$C$9</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
-                  <bgColor rgb="FF92D050"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>E2:E27</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{659722BC-F2F4-4942-880F-B665D77C82FE}">
-            <xm:f>NOT(ISERROR(SEARCH(Legendas!$C$7,F2)))</xm:f>
-            <xm:f>Legendas!$C$7</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="9" tint="0.39994506668294322"/>
+                  <bgColor rgb="FFFF0000"/>
                 </patternFill>
               </fill>
             </x14:dxf>
@@ -1482,18 +2665,18 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{247A90A8-51E8-41C3-9472-4F7E573E1980}">
-            <xm:f>NOT(ISERROR(SEARCH(Legendas!$C$9,F2)))</xm:f>
-            <xm:f>Legendas!$C$9</xm:f>
+          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{659722BC-F2F4-4942-880F-B665D77C82FE}">
+            <xm:f>NOT(ISERROR(SEARCH(Legendas!$C$7,F2)))</xm:f>
+            <xm:f>Legendas!$C$7</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
-                  <bgColor rgb="FFFF0000"/>
+                  <bgColor theme="9" tint="0.39994506668294322"/>
                 </patternFill>
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>F2:F27</xm:sqref>
+          <xm:sqref>F2:F85</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1503,19 +2686,19 @@
           <x14:formula1>
             <xm:f>Legendas!$C$2:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E27</xm:sqref>
+          <xm:sqref>E2:E85</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6A99346B-FB48-4F66-936C-FBDDB906B6F5}">
           <x14:formula1>
             <xm:f>Legendas!$C$7:$C$9</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F27</xm:sqref>
+          <xm:sqref>F2:F85</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{796B1647-1352-4E89-97DE-35C1550C744C}">
           <x14:formula1>
             <xm:f>Legendas!$H$2:$H$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D27</xm:sqref>
+          <xm:sqref>D2:D85</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>